<commit_message>
Complex to MySql WIP
</commit_message>
<xml_diff>
--- a/app/MLS_SpreadSheet_FieldsList.xlsx
+++ b/app/MLS_SpreadSheet_FieldsList.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="210">
   <si>
     <t>PicCount</t>
   </si>
@@ -650,6 +650,9 @@
   </si>
   <si>
     <t>StrataFee: 21,</t>
+  </si>
+  <si>
+    <t>MaintenanceFeeInclude</t>
   </si>
 </sst>
 </file>
@@ -3101,10 +3104,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R96"/>
+  <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="E73" workbookViewId="0">
+      <selection activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6957,16 +6960,28 @@
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H96">
+      <c r="H96" s="17">
         <v>93</v>
       </c>
-      <c r="I96">
+      <c r="I96" s="17">
         <v>91</v>
       </c>
-      <c r="J96" t="s">
+      <c r="J96" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="K96" s="17"/>
+    </row>
+    <row r="97" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H97">
+        <v>94</v>
+      </c>
+      <c r="I97">
+        <v>92</v>
+      </c>
+      <c r="J97" t="s">
         <v>196</v>
       </c>
-      <c r="K96" t="s">
+      <c r="K97" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sync Community to WP
</commit_message>
<xml_diff>
--- a/app/MLS_SpreadSheet_FieldsList.xlsx
+++ b/app/MLS_SpreadSheet_FieldsList.xlsx
@@ -1,29 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\ChromeX\MLSHelper\app\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B835EEF1-C0BC-4C42-BF5B-A35582DA2D7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="150" windowWidth="27270" windowHeight="16965" activeTab="1"/>
+    <workbookView xWindow="-29010" yWindow="30" windowWidth="29040" windowHeight="17400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Spreadsheet View Fields" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="211">
   <si>
     <t>PicCount</t>
   </si>
@@ -653,12 +651,15 @@
   </si>
   <si>
     <t>MaintenanceFeeInclude</t>
+  </si>
+  <si>
+    <t>List Desig Agt 1 - Active Listings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -826,7 +827,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1027,6 +1028,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1276,7 +1283,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1313,6 +1320,7 @@
     <xf numFmtId="0" fontId="20" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1414,7 +1422,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1447,9 +1455,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1482,6 +1507,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1657,7 +1699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3103,11 +3145,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E73" workbookViewId="0">
-      <selection activeCell="J96" sqref="J96"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J85" sqref="J85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,7 +3159,7 @@
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" customWidth="1"/>
     <col min="11" max="11" width="47.7109375" customWidth="1"/>
     <col min="15" max="15" width="23.28515625" customWidth="1"/>
     <col min="16" max="16" width="9.7109375" customWidth="1"/>
@@ -6029,7 +6071,7 @@
         <v>58</v>
       </c>
       <c r="J63" s="17" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="K63" s="17" t="s">
         <v>143</v>
@@ -6615,7 +6657,7 @@
       <c r="I76">
         <v>71</v>
       </c>
-      <c r="J76" t="s">
+      <c r="J76" s="28" t="s">
         <v>63</v>
       </c>
       <c r="K76" t="s">
@@ -6731,14 +6773,14 @@
       <c r="I80" s="17">
         <v>75</v>
       </c>
-      <c r="J80" s="17" t="s">
+      <c r="J80" s="28" t="s">
         <v>48</v>
       </c>
       <c r="K80" s="17" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>74</v>
       </c>
@@ -6763,21 +6805,24 @@
         <v>168</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H82">
         <v>79</v>
       </c>
       <c r="I82">
         <v>77</v>
       </c>
-      <c r="J82" t="s">
+      <c r="J82" s="28" t="s">
         <v>182</v>
       </c>
       <c r="K82" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H83">
         <v>80</v>
       </c>
@@ -6791,7 +6836,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H84">
         <v>81</v>
       </c>
@@ -6805,7 +6850,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H85" s="17">
         <v>82</v>
       </c>
@@ -6819,7 +6864,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H86" s="17">
         <v>83</v>
       </c>
@@ -6833,7 +6878,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H87" s="17">
         <v>84</v>
       </c>
@@ -6847,7 +6892,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H88" s="17">
         <v>85</v>
       </c>
@@ -6861,7 +6906,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H89" s="17">
         <v>86</v>
       </c>
@@ -6875,7 +6920,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H90" s="17">
         <v>87</v>
       </c>
@@ -6889,7 +6934,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H91" s="17">
         <v>88</v>
       </c>
@@ -6903,7 +6948,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H92" s="17">
         <v>89</v>
       </c>
@@ -6917,7 +6962,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H93" s="17">
         <v>90</v>
       </c>
@@ -6931,7 +6976,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H94" s="17">
         <v>91</v>
       </c>
@@ -6945,7 +6990,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H95" s="17">
         <v>92</v>
       </c>
@@ -6959,7 +7004,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H96" s="17">
         <v>93</v>
       </c>

</xml_diff>